<commit_message>
setting up LCI modeling for varying parameters
</commit_message>
<xml_diff>
--- a/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
+++ b/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1DA58C-967A-4D4B-8EA7-53FD2EFE42CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C517E3-6473-4A67-A472-C9A7B8F41BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="364">
   <si>
     <t>Agg_CF_irri</t>
   </si>
@@ -1110,6 +1110,12 @@
   </si>
   <si>
     <t>Sal</t>
+  </si>
+  <si>
+    <t>Salton Sea</t>
+  </si>
+  <si>
+    <t>Upper Rhine Graben</t>
   </si>
 </sst>
 </file>
@@ -1702,12 +1708,12 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.86328125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="111.86328125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="4" width="22.73046875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="111.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
@@ -1752,7 +1758,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="42.75">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="15" t="s">
         <v>290</v>
       </c>
@@ -1816,18 +1822,18 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F285" sqref="F285"/>
+      <selection pane="bottomLeft" activeCell="A285" sqref="A285"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1328125" style="1"/>
-    <col min="5" max="5" width="9.1328125" customWidth="1"/>
-    <col min="6" max="6" width="14.73046875" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5997,7 +6003,7 @@
     </row>
     <row r="284" spans="1:6">
       <c r="A284" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B284" s="1">
         <v>0.9</v>
@@ -6014,7 +6020,7 @@
     </row>
     <row r="285" spans="1:6">
       <c r="A285" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B285" s="1">
         <v>6.2</v>
@@ -6043,7 +6049,7 @@
       <selection activeCell="L22" sqref="L22:L48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="20" t="s">
@@ -6909,18 +6915,18 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="37" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="37" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="14.65" thickBot="1">
+    <row r="1" spans="1:37" ht="15.75" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="14.65" thickBot="1">
+    <row r="2" spans="1:37" ht="15.75" thickBot="1">
       <c r="B2" s="27" t="s">
         <v>229</v>
       </c>
@@ -30928,7 +30934,7 @@
         <v>3.4306674594570494</v>
       </c>
     </row>
-    <row r="216" spans="1:37" ht="14.65" thickBot="1">
+    <row r="216" spans="1:37" ht="15.75" thickBot="1">
       <c r="A216" t="s">
         <v>209</v>
       </c>
@@ -31135,11 +31141,11 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="3" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
Regionalization of AWARE combined with created db
</commit_message>
<xml_diff>
--- a/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
+++ b/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4D42E-1397-4D08-BB62-325D872EF2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E14381-9460-45FF-95D5-483419190280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -1728,12 +1728,12 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="111.85546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.86328125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="111.86328125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
@@ -1778,7 +1778,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="42.75">
       <c r="A8" s="15" t="s">
         <v>290</v>
       </c>
@@ -1841,19 +1841,19 @@
   <dimension ref="A1:L290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A290" sqref="A290"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A285" sqref="A285"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1328125" style="1"/>
+    <col min="5" max="5" width="9.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.73046875" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" customWidth="1"/>
+    <col min="8" max="8" width="14.86328125" customWidth="1"/>
+    <col min="9" max="9" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6161,7 +6161,7 @@
       <selection activeCell="L22" sqref="L22:L48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="20" t="s">
@@ -7027,18 +7027,18 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="37" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="2" max="37" width="9.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" thickBot="1">
+    <row r="1" spans="1:37" ht="14.65" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" thickBot="1">
+    <row r="2" spans="1:37" ht="14.65" thickBot="1">
       <c r="B2" s="27" t="s">
         <v>229</v>
       </c>
@@ -31046,7 +31046,7 @@
         <v>3.4306674594570494</v>
       </c>
     </row>
-    <row r="216" spans="1:37" ht="15.75" thickBot="1">
+    <row r="216" spans="1:37" ht="14.65" thickBot="1">
       <c r="A216" t="s">
         <v>209</v>
       </c>
@@ -31253,11 +31253,11 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
     <col min="2" max="3" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
update of visualization class
</commit_message>
<xml_diff>
--- a/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
+++ b/data/AWARE_country_regions_Corrected_online_20230113-1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E5D801-979F-4505-B923-8BDB99E14B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72FEFA6-2F48-49C0-BA05-E58D9FE87DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="14400" windowHeight="7282" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -1177,9 +1177,6 @@
     <t>Salar de Antofalla</t>
   </si>
   <si>
-    <t>Salar de Pocito</t>
-  </si>
-  <si>
     <t>Pocuelos</t>
   </si>
   <si>
@@ -1211,6 +1208,9 @@
   </si>
   <si>
     <t>Sal de los Angeles</t>
+  </si>
+  <si>
+    <t>Salar de Pocitos</t>
   </si>
 </sst>
 </file>
@@ -1923,8 +1923,8 @@
   <dimension ref="A1:L315"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
+      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="290" spans="1:6">
       <c r="A290" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B290" s="1">
         <v>48.5</v>
@@ -6432,7 +6432,7 @@
     </row>
     <row r="302" spans="1:6">
       <c r="A302" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B302" s="1">
         <v>2.7</v>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="305" spans="1:6">
       <c r="A305" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="B305" s="1">
         <v>5</v>
@@ -6499,12 +6499,12 @@
       </c>
       <c r="F305" t="str">
         <f t="shared" si="1"/>
-        <v>Salar de Pocito</v>
+        <v>Salar de Pocitos</v>
       </c>
     </row>
     <row r="306" spans="1:6">
       <c r="A306" s="24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B306" s="1">
         <v>5</v>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="308" spans="1:6">
       <c r="A308" s="24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B308" s="1">
         <v>97.5</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="309" spans="1:6">
       <c r="A309" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B309" s="1">
         <v>2.8</v>
@@ -6576,7 +6576,7 @@
     </row>
     <row r="310" spans="1:6">
       <c r="A310" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B310" s="1">
         <v>0.6</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="311" spans="1:6">
       <c r="A311" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B311" s="1">
         <v>22</v>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="312" spans="1:6">
       <c r="A312" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B312" s="1">
         <v>22</v>
@@ -6630,7 +6630,7 @@
     </row>
     <row r="313" spans="1:6">
       <c r="A313" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B313" s="1">
         <v>100</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="314" spans="1:6">
       <c r="A314" s="24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B314" s="1">
         <v>97</v>
@@ -6666,7 +6666,7 @@
     </row>
     <row r="315" spans="1:6">
       <c r="A315" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B315" s="1">
         <v>15.2</v>

</xml_diff>